<commit_message>
Elle giriş ve hata çözümlemesi
</commit_message>
<xml_diff>
--- a/kitaplar.xlsx
+++ b/kitaplar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Title</t>
   </si>
@@ -22,22 +22,28 @@
     <t>Authors</t>
   </si>
   <si>
+    <t>Atomik Aliskanliklar - Kücük Degisikler Büyük Sonuclar - Kötü Aliskanliklardan Kurtulup Iyi Aliskanliklar Edinmek Icin Kolay ve Etkisi Kanitlanmis Bir Yöntem</t>
+  </si>
+  <si>
+    <t>Scikit-Learn Makine Ogrenimi</t>
+  </si>
+  <si>
     <t>Ikigai - Uygulama Rehberi - Japonlarin Uzun ve Mutlu Yasam Sirrini Hayata Gecirin</t>
   </si>
   <si>
     <t>İnsan tabiatını tanıma</t>
   </si>
   <si>
-    <t>Atomik Aliskanliklar - Kücük Degisikler Büyük Sonuclar - Kötü Aliskanliklardan Kurtulup Iyi Aliskanliklar Edinmek Icin Kolay ve Etkisi Kanitlanmis Bir Yöntem</t>
+    <t>['James Clear']</t>
+  </si>
+  <si>
+    <t>Oreilly</t>
   </si>
   <si>
     <t>['Hector Garcia', 'Francesc Miralles']</t>
   </si>
   <si>
     <t>['Alfred Adler']</t>
-  </si>
-  <si>
-    <t>['James Clear']</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -428,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -439,7 +445,18 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Süreç denendi bulunan hatalar not alındı.
</commit_message>
<xml_diff>
--- a/kitaplar.xlsx
+++ b/kitaplar.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Title</t>
   </si>
@@ -22,16 +22,40 @@
     <t>Authors</t>
   </si>
   <si>
-    <t>Adalet adına</t>
-  </si>
-  <si>
-    <t>Gazi Mustafa Kemal Atatürk</t>
-  </si>
-  <si>
-    <t>['Nancy Taylor Rosenberg', 'İbrahim Kırkaǧaçlıoǧlu']</t>
-  </si>
-  <si>
-    <t>['İlber Ortaylı']</t>
+    <t>Anadolu notları</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1703 Edirne vakası</t>
+  </si>
+  <si>
+    <t>Halide Edib Adivar</t>
+  </si>
+  <si>
+    <t>Karmasik Duygular</t>
+  </si>
+  <si>
+    <t>Tarihte ilginç gerçekler</t>
+  </si>
+  <si>
+    <t>['Reşat Nuri Güntekin']</t>
+  </si>
+  <si>
+    <t>['George Orwell']</t>
+  </si>
+  <si>
+    <t>['Tahir Sevinç', 'Behset Karaca', 'Süleyman Demirel Üniversitesi. Sosyal Bilimler Enstitüsü. Tarih Anabilim Dalı']</t>
+  </si>
+  <si>
+    <t>['Sinekli Bakkal']</t>
+  </si>
+  <si>
+    <t>['Stefan Zweig']</t>
+  </si>
+  <si>
+    <t>['']</t>
   </si>
 </sst>
 </file>
@@ -389,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,7 +435,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -422,7 +446,51 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>